<commit_message>
some improvements, still more to go
</commit_message>
<xml_diff>
--- a/data/raw/farmhub_raw_2023.xlsx
+++ b/data/raw/farmhub_raw_2023.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ey239/Github/IMT/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B0B0290-3E4F-F842-B71B-E1CE3C369760}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6366205F-39B7-7C4D-BC12-11BFBF53F73A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18720" yWindow="-23740" windowWidth="34160" windowHeight="21100" xr2:uid="{8C11EFA4-E327-134C-9653-82A048CD8AB5}"/>
+    <workbookView xWindow="4240" yWindow="-21000" windowWidth="34160" windowHeight="21000" xr2:uid="{8C11EFA4-E327-134C-9653-82A048CD8AB5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -650,7 +650,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1CD38F1-6215-FB42-993C-AE85EFD73AEA}">
   <dimension ref="A1:P37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="J40" sqref="J40"/>
     </sheetView>
   </sheetViews>
@@ -670,6 +670,7 @@
     <col min="12" max="12" width="13" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="17" x14ac:dyDescent="0.2">

</xml_diff>